<commit_message>
check moth counts with all other variables
</commit_message>
<xml_diff>
--- a/Input/2023_2024_all_moth_counts.xlsx
+++ b/Input/2023_2024_all_moth_counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Noa/Documents/Documents - MacBook Air/PhD/R:Stats:GIS/RStudio/R_Workspace/Pheromone_trap_code/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396B5F01-B27F-3C40-8046-A43AAF99E9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{820BEA8E-6E59-2D42-8667-2F0B78F28BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="660" windowWidth="28660" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="540" windowWidth="28660" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - 2024_consolidated_mot" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="398">
   <si>
     <t>patch_name</t>
   </si>
@@ -1078,17 +1078,174 @@
   </si>
   <si>
     <t>Count of actual moths (whole and parts) from traps, some counts are partial and some complete (for 2023, traps with no count, due to high or very high muck, were estimated to have at least 30 moths (high) or 50 moths) (very high)</t>
+  </si>
+  <si>
+    <t>Tree Species:</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Bouleau à papier (blanc)</t>
+  </si>
+  <si>
+    <t>Paper Birch (White)</t>
+  </si>
+  <si>
+    <t>Bouleau gris (à feuilles de peuplier)</t>
+  </si>
+  <si>
+    <t>gray birch (poplar-leaved)</t>
+  </si>
+  <si>
+    <t>Bouleau jaune</t>
+  </si>
+  <si>
+    <t>Yellow Birch</t>
+  </si>
+  <si>
+    <t>Chêne rouge</t>
+  </si>
+  <si>
+    <t>red oak</t>
+  </si>
+  <si>
+    <t>épinette blanche</t>
+  </si>
+  <si>
+    <t>White Spruce</t>
+  </si>
+  <si>
+    <t>Épinette rouge</t>
+  </si>
+  <si>
+    <t>Red Spruce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Érable à sucre </t>
+  </si>
+  <si>
+    <t>sugar maple</t>
+  </si>
+  <si>
+    <t>Érable rouge</t>
+  </si>
+  <si>
+    <t>red maple</t>
+  </si>
+  <si>
+    <t>Feuillus intolérants à l'ombre</t>
+  </si>
+  <si>
+    <t>Shade-Intolerant Hardwoods</t>
+  </si>
+  <si>
+    <t>Feuillus non commerciaux</t>
+  </si>
+  <si>
+    <t>non-commercial hardwoods</t>
+  </si>
+  <si>
+    <t>Feuillus tolérants à l'ombre</t>
+  </si>
+  <si>
+    <t>Shade-Tolerant Hardwoods shade</t>
+  </si>
+  <si>
+    <t>Frêne noir</t>
+  </si>
+  <si>
+    <t>black ash</t>
+  </si>
+  <si>
+    <t>Frênes</t>
+  </si>
+  <si>
+    <t>Ash</t>
+  </si>
+  <si>
+    <t>Hêtre à grandes feuilles</t>
+  </si>
+  <si>
+    <t>American beech</t>
+  </si>
+  <si>
+    <t>Ormes</t>
+  </si>
+  <si>
+    <t>elms</t>
+  </si>
+  <si>
+    <t>Peupliers naturels</t>
+  </si>
+  <si>
+    <t>Natural Poplars</t>
+  </si>
+  <si>
+    <t>Pin blanc</t>
+  </si>
+  <si>
+    <t>White Pine</t>
+  </si>
+  <si>
+    <t>Pin rouge</t>
+  </si>
+  <si>
+    <t>red pine</t>
+  </si>
+  <si>
+    <t>Pruche du Canada (de l'Est)</t>
+  </si>
+  <si>
+    <t>Eastern Hemlock</t>
+  </si>
+  <si>
+    <t>Résineux indéterminés</t>
+  </si>
+  <si>
+    <t>Indeterminate Softwood</t>
+  </si>
+  <si>
+    <t>Sapin baumier</t>
+  </si>
+  <si>
+    <t>Balsam Fir</t>
+  </si>
+  <si>
+    <t>Tilleul d'Amérique</t>
+  </si>
+  <si>
+    <t>American basswood</t>
+  </si>
+  <si>
+    <t>oak_pine</t>
+  </si>
+  <si>
+    <t>pine_oak</t>
+  </si>
+  <si>
+    <t>maple_pine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1168,7 +1325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1181,8 +1338,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1246,158 +1415,199 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1495,10 +1705,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>283380</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>11546</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1922835</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>80819</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2582,8 +2792,8 @@
   <dimension ref="A1:S256"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2691,11 +2901,15 @@
       <c r="H2" s="14">
         <v>0</v>
       </c>
-      <c r="I2" s="14"/>
+      <c r="I2" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J2" s="14">
         <v>14</v>
       </c>
-      <c r="K2" s="14"/>
+      <c r="K2" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L2" s="12" t="s">
         <v>17</v>
       </c>
@@ -2743,11 +2957,15 @@
       <c r="H3" s="14">
         <v>0</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J3" s="14">
         <v>6.4</v>
       </c>
-      <c r="K3" s="14"/>
+      <c r="K3" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L3" s="12" t="s">
         <v>21</v>
       </c>
@@ -2795,11 +3013,15 @@
       <c r="H4" s="14">
         <v>0</v>
       </c>
-      <c r="I4" s="14"/>
+      <c r="I4" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J4" s="14">
         <v>8.6</v>
       </c>
-      <c r="K4" s="14"/>
+      <c r="K4" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L4" s="12" t="s">
         <v>23</v>
       </c>
@@ -2847,11 +3069,15 @@
       <c r="H5" s="14">
         <v>0</v>
       </c>
-      <c r="I5" s="14"/>
+      <c r="I5" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J5" s="14">
         <v>8.6</v>
       </c>
-      <c r="K5" s="14"/>
+      <c r="K5" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L5" s="12" t="s">
         <v>24</v>
       </c>
@@ -2899,11 +3125,15 @@
       <c r="H6" s="14">
         <v>0</v>
       </c>
-      <c r="I6" s="14"/>
+      <c r="I6" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J6" s="14">
         <v>8.6</v>
       </c>
-      <c r="K6" s="14"/>
+      <c r="K6" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L6" s="12" t="s">
         <v>25</v>
       </c>
@@ -2951,11 +3181,15 @@
       <c r="H7" s="14">
         <v>0</v>
       </c>
-      <c r="I7" s="14"/>
+      <c r="I7" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J7" s="14">
         <v>11.7</v>
       </c>
-      <c r="K7" s="14"/>
+      <c r="K7" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L7" s="12" t="s">
         <v>26</v>
       </c>
@@ -3003,11 +3237,15 @@
       <c r="H8" s="14">
         <v>0</v>
       </c>
-      <c r="I8" s="14"/>
+      <c r="I8" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J8" s="14">
         <v>11.7</v>
       </c>
-      <c r="K8" s="14"/>
+      <c r="K8" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L8" s="12" t="s">
         <v>27</v>
       </c>
@@ -3055,11 +3293,15 @@
       <c r="H9" s="14">
         <v>0</v>
       </c>
-      <c r="I9" s="14"/>
+      <c r="I9" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J9" s="14">
         <v>11.7</v>
       </c>
-      <c r="K9" s="14"/>
+      <c r="K9" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L9" s="12" t="s">
         <v>28</v>
       </c>
@@ -3107,11 +3349,15 @@
       <c r="H10" s="14">
         <v>0.1</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J10" s="14">
         <v>8.9</v>
       </c>
-      <c r="K10" s="14"/>
+      <c r="K10" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L10" s="12" t="s">
         <v>31</v>
       </c>
@@ -3159,11 +3405,15 @@
       <c r="H11" s="14">
         <v>0.1</v>
       </c>
-      <c r="I11" s="14"/>
+      <c r="I11" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J11" s="14">
         <v>8.9</v>
       </c>
-      <c r="K11" s="14"/>
+      <c r="K11" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L11" s="12" t="s">
         <v>32</v>
       </c>
@@ -3211,11 +3461,15 @@
       <c r="H12" s="14">
         <v>0.1</v>
       </c>
-      <c r="I12" s="14"/>
+      <c r="I12" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J12" s="14">
         <v>8.9</v>
       </c>
-      <c r="K12" s="14"/>
+      <c r="K12" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L12" s="12" t="s">
         <v>33</v>
       </c>
@@ -3263,11 +3517,15 @@
       <c r="H13" s="14">
         <v>0.1</v>
       </c>
-      <c r="I13" s="14"/>
+      <c r="I13" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J13" s="14">
         <v>8.9</v>
       </c>
-      <c r="K13" s="14"/>
+      <c r="K13" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L13" s="12" t="s">
         <v>34</v>
       </c>
@@ -3315,11 +3573,15 @@
       <c r="H14" s="15">
         <v>0</v>
       </c>
-      <c r="I14" s="15"/>
+      <c r="I14" s="15" t="s">
+        <v>313</v>
+      </c>
       <c r="J14" s="14">
         <v>14</v>
       </c>
-      <c r="K14" s="14"/>
+      <c r="K14" s="14">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="L14" s="12" t="s">
         <v>37</v>
       </c>
@@ -3367,11 +3629,15 @@
       <c r="H15" s="14">
         <v>0</v>
       </c>
-      <c r="I15" s="14"/>
+      <c r="I15" s="14" t="s">
+        <v>318</v>
+      </c>
       <c r="J15" s="14">
         <v>4.8</v>
       </c>
-      <c r="K15" s="14"/>
+      <c r="K15" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L15" s="12" t="s">
         <v>40</v>
       </c>
@@ -3419,11 +3685,15 @@
       <c r="H16" s="14">
         <v>0</v>
       </c>
-      <c r="I16" s="14"/>
+      <c r="I16" s="14" t="s">
+        <v>318</v>
+      </c>
       <c r="J16" s="14">
         <v>4.8</v>
       </c>
-      <c r="K16" s="14"/>
+      <c r="K16" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L16" s="12" t="s">
         <v>41</v>
       </c>
@@ -3471,11 +3741,15 @@
       <c r="H17" s="14">
         <v>0</v>
       </c>
-      <c r="I17" s="14"/>
+      <c r="I17" s="14" t="s">
+        <v>318</v>
+      </c>
       <c r="J17" s="14">
         <v>4.8</v>
       </c>
-      <c r="K17" s="14"/>
+      <c r="K17" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L17" s="12" t="s">
         <v>42</v>
       </c>
@@ -3523,11 +3797,15 @@
       <c r="H18" s="14">
         <v>0</v>
       </c>
-      <c r="I18" s="14"/>
+      <c r="I18" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J18" s="14">
         <v>8.5</v>
       </c>
-      <c r="K18" s="14"/>
+      <c r="K18" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L18" s="12" t="s">
         <v>43</v>
       </c>
@@ -3575,11 +3853,15 @@
       <c r="H19" s="14">
         <v>0</v>
       </c>
-      <c r="I19" s="14"/>
+      <c r="I19" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J19" s="14">
         <v>8.5</v>
       </c>
-      <c r="K19" s="14"/>
+      <c r="K19" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L19" s="12" t="s">
         <v>44</v>
       </c>
@@ -3627,11 +3909,15 @@
       <c r="H20" s="14">
         <v>0</v>
       </c>
-      <c r="I20" s="14"/>
+      <c r="I20" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J20" s="14">
         <v>8.5</v>
       </c>
-      <c r="K20" s="14"/>
+      <c r="K20" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L20" s="12" t="s">
         <v>45</v>
       </c>
@@ -3679,11 +3965,15 @@
       <c r="H21" s="14">
         <v>0</v>
       </c>
-      <c r="I21" s="14"/>
+      <c r="I21" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J21" s="14">
         <v>8.5</v>
       </c>
-      <c r="K21" s="14"/>
+      <c r="K21" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L21" s="12" t="s">
         <v>46</v>
       </c>
@@ -3731,11 +4021,15 @@
       <c r="H22" s="14">
         <v>0.1</v>
       </c>
-      <c r="I22" s="14"/>
+      <c r="I22" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J22" s="14">
         <v>5.7</v>
       </c>
-      <c r="K22" s="14"/>
+      <c r="K22" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L22" s="12" t="s">
         <v>49</v>
       </c>
@@ -3783,11 +4077,15 @@
       <c r="H23" s="14">
         <v>0.1</v>
       </c>
-      <c r="I23" s="14"/>
+      <c r="I23" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J23" s="14">
         <v>5.7</v>
       </c>
-      <c r="K23" s="14"/>
+      <c r="K23" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L23" s="12" t="s">
         <v>50</v>
       </c>
@@ -3835,11 +4133,15 @@
       <c r="H24" s="14">
         <v>0.1</v>
       </c>
-      <c r="I24" s="14"/>
+      <c r="I24" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J24" s="14">
         <v>5.7</v>
       </c>
-      <c r="K24" s="14"/>
+      <c r="K24" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L24" s="12" t="s">
         <v>51</v>
       </c>
@@ -3887,11 +4189,15 @@
       <c r="H25" s="14">
         <v>0.2</v>
       </c>
-      <c r="I25" s="14"/>
+      <c r="I25" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J25" s="14">
         <v>7.6</v>
       </c>
-      <c r="K25" s="14"/>
+      <c r="K25" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L25" s="12" t="s">
         <v>53</v>
       </c>
@@ -3939,11 +4245,15 @@
       <c r="H26" s="14">
         <v>0.2</v>
       </c>
-      <c r="I26" s="14"/>
+      <c r="I26" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J26" s="14">
         <v>7.6</v>
       </c>
-      <c r="K26" s="14"/>
+      <c r="K26" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L26" s="12" t="s">
         <v>54</v>
       </c>
@@ -3991,11 +4301,15 @@
       <c r="H27" s="14">
         <v>0.2</v>
       </c>
-      <c r="I27" s="14"/>
+      <c r="I27" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J27" s="14">
         <v>7.6</v>
       </c>
-      <c r="K27" s="14"/>
+      <c r="K27" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L27" s="12" t="s">
         <v>55</v>
       </c>
@@ -4043,11 +4357,15 @@
       <c r="H28" s="14">
         <v>0.2</v>
       </c>
-      <c r="I28" s="14"/>
+      <c r="I28" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J28" s="14">
         <v>7.6</v>
       </c>
-      <c r="K28" s="14"/>
+      <c r="K28" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L28" s="12" t="s">
         <v>56</v>
       </c>
@@ -4095,11 +4413,15 @@
       <c r="H29" s="14">
         <v>0.7</v>
       </c>
-      <c r="I29" s="14"/>
+      <c r="I29" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J29" s="14">
         <v>3.8</v>
       </c>
-      <c r="K29" s="14"/>
+      <c r="K29" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L29" s="12" t="s">
         <v>57</v>
       </c>
@@ -4147,11 +4469,15 @@
       <c r="H30" s="14">
         <v>0.4</v>
       </c>
-      <c r="I30" s="14"/>
+      <c r="I30" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J30" s="14">
         <v>3.5</v>
       </c>
-      <c r="K30" s="14"/>
+      <c r="K30" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L30" s="12" t="s">
         <v>60</v>
       </c>
@@ -4199,11 +4525,15 @@
       <c r="H31" s="14">
         <v>0.4</v>
       </c>
-      <c r="I31" s="14"/>
+      <c r="I31" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J31" s="14">
         <v>3.5</v>
       </c>
-      <c r="K31" s="14"/>
+      <c r="K31" s="14">
+        <v>12.4</v>
+      </c>
       <c r="L31" s="12" t="s">
         <v>61</v>
       </c>
@@ -4251,11 +4581,15 @@
       <c r="H32" s="14">
         <v>0</v>
       </c>
-      <c r="I32" s="14"/>
+      <c r="I32" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J32" s="14">
         <v>5.7</v>
       </c>
-      <c r="K32" s="14"/>
+      <c r="K32" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L32" s="12" t="s">
         <v>64</v>
       </c>
@@ -4303,11 +4637,15 @@
       <c r="H33" s="14">
         <v>0.1</v>
       </c>
-      <c r="I33" s="14"/>
+      <c r="I33" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J33" s="14">
         <v>7.5</v>
       </c>
-      <c r="K33" s="14"/>
+      <c r="K33" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L33" s="12" t="s">
         <v>66</v>
       </c>
@@ -4355,11 +4693,15 @@
       <c r="H34" s="14">
         <v>0.1</v>
       </c>
-      <c r="I34" s="14"/>
+      <c r="I34" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J34" s="14">
         <v>7.5</v>
       </c>
-      <c r="K34" s="14"/>
+      <c r="K34" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L34" s="12" t="s">
         <v>68</v>
       </c>
@@ -4407,11 +4749,15 @@
       <c r="H35" s="14">
         <v>0</v>
       </c>
-      <c r="I35" s="14"/>
+      <c r="I35" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J35" s="14">
         <v>4.8</v>
       </c>
-      <c r="K35" s="14"/>
+      <c r="K35" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L35" s="12" t="s">
         <v>69</v>
       </c>
@@ -4459,11 +4805,15 @@
       <c r="H36" s="14">
         <v>0</v>
       </c>
-      <c r="I36" s="14"/>
+      <c r="I36" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J36" s="14">
         <v>4.8</v>
       </c>
-      <c r="K36" s="14"/>
+      <c r="K36" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L36" s="12" t="s">
         <v>70</v>
       </c>
@@ -4511,11 +4861,15 @@
       <c r="H37" s="14">
         <v>0.4</v>
       </c>
-      <c r="I37" s="14"/>
+      <c r="I37" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J37" s="14">
         <v>9.6999999999999993</v>
       </c>
-      <c r="K37" s="14"/>
+      <c r="K37" s="14">
+        <v>1282</v>
+      </c>
       <c r="L37" s="12" t="s">
         <v>72</v>
       </c>
@@ -4563,11 +4917,15 @@
       <c r="H38" s="14">
         <v>0.4</v>
       </c>
-      <c r="I38" s="14"/>
+      <c r="I38" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J38" s="14">
         <v>9.6999999999999993</v>
       </c>
-      <c r="K38" s="14"/>
+      <c r="K38" s="14">
+        <v>1282</v>
+      </c>
       <c r="L38" s="12" t="s">
         <v>73</v>
       </c>
@@ -4615,11 +4973,15 @@
       <c r="H39" s="14">
         <v>0.4</v>
       </c>
-      <c r="I39" s="14"/>
+      <c r="I39" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J39" s="14">
         <v>7.6</v>
       </c>
-      <c r="K39" s="14"/>
+      <c r="K39" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L39" s="12" t="s">
         <v>74</v>
       </c>
@@ -4667,11 +5029,15 @@
       <c r="H40" s="14">
         <v>0.4</v>
       </c>
-      <c r="I40" s="14"/>
+      <c r="I40" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J40" s="14">
         <v>7.6</v>
       </c>
-      <c r="K40" s="14"/>
+      <c r="K40" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L40" s="12" t="s">
         <v>75</v>
       </c>
@@ -4719,11 +5085,15 @@
       <c r="H41" s="14">
         <v>0.4</v>
       </c>
-      <c r="I41" s="14"/>
+      <c r="I41" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J41" s="14">
         <v>7.6</v>
       </c>
-      <c r="K41" s="14"/>
+      <c r="K41" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L41" s="12" t="s">
         <v>76</v>
       </c>
@@ -4771,11 +5141,15 @@
       <c r="H42" s="14">
         <v>0.6</v>
       </c>
-      <c r="I42" s="14"/>
+      <c r="I42" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J42" s="14">
         <v>12.2</v>
       </c>
-      <c r="K42" s="14"/>
+      <c r="K42" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L42" s="12" t="s">
         <v>78</v>
       </c>
@@ -4823,11 +5197,15 @@
       <c r="H43" s="14">
         <v>0.6</v>
       </c>
-      <c r="I43" s="14"/>
+      <c r="I43" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J43" s="14">
         <v>12.2</v>
       </c>
-      <c r="K43" s="14"/>
+      <c r="K43" s="14">
+        <v>16.3</v>
+      </c>
       <c r="L43" s="12" t="s">
         <v>79</v>
       </c>
@@ -4875,11 +5253,15 @@
       <c r="H44" s="14">
         <v>0.8</v>
       </c>
-      <c r="I44" s="14"/>
+      <c r="I44" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J44" s="14">
         <v>8.1999999999999993</v>
       </c>
-      <c r="K44" s="14"/>
+      <c r="K44" s="14">
+        <v>1282</v>
+      </c>
       <c r="L44" s="12" t="s">
         <v>81</v>
       </c>
@@ -4927,11 +5309,15 @@
       <c r="H45" s="14">
         <v>0.8</v>
       </c>
-      <c r="I45" s="14"/>
+      <c r="I45" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J45" s="14">
         <v>8.1999999999999993</v>
       </c>
-      <c r="K45" s="14"/>
+      <c r="K45" s="14">
+        <v>1282</v>
+      </c>
       <c r="L45" s="12" t="s">
         <v>82</v>
       </c>
@@ -4979,11 +5365,15 @@
       <c r="H46" s="14">
         <v>0.4</v>
       </c>
-      <c r="I46" s="14"/>
+      <c r="I46" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J46" s="14">
         <v>8.6999999999999993</v>
       </c>
-      <c r="K46" s="14"/>
+      <c r="K46" s="14">
+        <v>1282</v>
+      </c>
       <c r="L46" s="12" t="s">
         <v>83</v>
       </c>
@@ -5031,11 +5421,15 @@
       <c r="H47" s="14">
         <v>0.4</v>
       </c>
-      <c r="I47" s="14"/>
+      <c r="I47" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J47" s="14">
         <v>8.6999999999999993</v>
       </c>
-      <c r="K47" s="14"/>
+      <c r="K47" s="14">
+        <v>1282</v>
+      </c>
       <c r="L47" s="12" t="s">
         <v>84</v>
       </c>
@@ -5083,11 +5477,15 @@
       <c r="H48" s="14">
         <v>0</v>
       </c>
-      <c r="I48" s="14"/>
+      <c r="I48" s="14" t="s">
+        <v>322</v>
+      </c>
       <c r="J48" s="14">
         <v>4.9000000000000004</v>
       </c>
-      <c r="K48" s="14"/>
+      <c r="K48" s="14">
+        <v>1282</v>
+      </c>
       <c r="L48" s="12" t="s">
         <v>86</v>
       </c>
@@ -5135,11 +5533,15 @@
       <c r="H49" s="14">
         <v>0</v>
       </c>
-      <c r="I49" s="14"/>
+      <c r="I49" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J49" s="14">
         <v>7.8</v>
       </c>
-      <c r="K49" s="14"/>
+      <c r="K49" s="14">
+        <v>1282</v>
+      </c>
       <c r="L49" s="12" t="s">
         <v>87</v>
       </c>
@@ -5187,11 +5589,15 @@
       <c r="H50" s="14">
         <v>0</v>
       </c>
-      <c r="I50" s="14"/>
+      <c r="I50" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J50" s="14">
         <v>7.8</v>
       </c>
-      <c r="K50" s="14"/>
+      <c r="K50" s="14">
+        <v>1282</v>
+      </c>
       <c r="L50" s="12" t="s">
         <v>88</v>
       </c>
@@ -5239,11 +5645,15 @@
       <c r="H51" s="14">
         <v>0</v>
       </c>
-      <c r="I51" s="14"/>
+      <c r="I51" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J51" s="14">
         <v>7.8</v>
       </c>
-      <c r="K51" s="14"/>
+      <c r="K51" s="14">
+        <v>1282</v>
+      </c>
       <c r="L51" s="12" t="s">
         <v>89</v>
       </c>
@@ -5291,11 +5701,15 @@
       <c r="H52" s="14">
         <v>0</v>
       </c>
-      <c r="I52" s="14"/>
+      <c r="I52" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J52" s="14">
         <v>7.8</v>
       </c>
-      <c r="K52" s="14"/>
+      <c r="K52" s="14">
+        <v>1282</v>
+      </c>
       <c r="L52" s="12" t="s">
         <v>90</v>
       </c>
@@ -5343,11 +5757,15 @@
       <c r="H53" s="14">
         <v>0.3</v>
       </c>
-      <c r="I53" s="14"/>
+      <c r="I53" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J53" s="14">
         <v>5.5</v>
       </c>
-      <c r="K53" s="14"/>
+      <c r="K53" s="14">
+        <v>1282</v>
+      </c>
       <c r="L53" s="12" t="s">
         <v>92</v>
       </c>
@@ -5395,11 +5813,15 @@
       <c r="H54" s="14">
         <v>0.3</v>
       </c>
-      <c r="I54" s="14"/>
+      <c r="I54" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J54" s="14">
         <v>5.5</v>
       </c>
-      <c r="K54" s="14"/>
+      <c r="K54" s="14">
+        <v>1282</v>
+      </c>
       <c r="L54" s="12" t="s">
         <v>93</v>
       </c>
@@ -5447,11 +5869,15 @@
       <c r="H55" s="14">
         <v>0.3</v>
       </c>
-      <c r="I55" s="14"/>
+      <c r="I55" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J55" s="14">
         <v>5.5</v>
       </c>
-      <c r="K55" s="14"/>
+      <c r="K55" s="14">
+        <v>1282</v>
+      </c>
       <c r="L55" s="12" t="s">
         <v>94</v>
       </c>
@@ -5499,11 +5925,15 @@
       <c r="H56" s="14">
         <v>0.3</v>
       </c>
-      <c r="I56" s="14"/>
+      <c r="I56" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J56" s="14">
         <v>5.5</v>
       </c>
-      <c r="K56" s="14"/>
+      <c r="K56" s="14">
+        <v>1282</v>
+      </c>
       <c r="L56" s="12" t="s">
         <v>95</v>
       </c>
@@ -5551,11 +5981,15 @@
       <c r="H57" s="14">
         <v>0.3</v>
       </c>
-      <c r="I57" s="14"/>
+      <c r="I57" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J57" s="14">
         <v>4.9000000000000004</v>
       </c>
-      <c r="K57" s="14"/>
+      <c r="K57" s="14">
+        <v>1282</v>
+      </c>
       <c r="L57" s="12" t="s">
         <v>96</v>
       </c>
@@ -5603,11 +6037,15 @@
       <c r="H58" s="14">
         <v>0.8</v>
       </c>
-      <c r="I58" s="14"/>
+      <c r="I58" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J58" s="14">
         <v>4.4000000000000004</v>
       </c>
-      <c r="K58" s="14"/>
+      <c r="K58" s="14">
+        <v>1282</v>
+      </c>
       <c r="L58" s="12" t="s">
         <v>97</v>
       </c>
@@ -5655,11 +6093,15 @@
       <c r="H59" s="14">
         <v>0.8</v>
       </c>
-      <c r="I59" s="14"/>
+      <c r="I59" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J59" s="14">
         <v>4.4000000000000004</v>
       </c>
-      <c r="K59" s="14"/>
+      <c r="K59" s="14">
+        <v>1282</v>
+      </c>
       <c r="L59" s="12" t="s">
         <v>98</v>
       </c>
@@ -5707,11 +6149,15 @@
       <c r="H60" s="14">
         <v>0.1</v>
       </c>
-      <c r="I60" s="14"/>
+      <c r="I60" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J60" s="14">
         <v>19.100000000000001</v>
       </c>
-      <c r="K60" s="14"/>
+      <c r="K60" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L60" s="12" t="s">
         <v>100</v>
       </c>
@@ -5759,11 +6205,15 @@
       <c r="H61" s="14">
         <v>0</v>
       </c>
-      <c r="I61" s="14"/>
+      <c r="I61" s="14" t="s">
+        <v>318</v>
+      </c>
       <c r="J61" s="14">
         <v>6.3</v>
       </c>
-      <c r="K61" s="14"/>
+      <c r="K61" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L61" s="12" t="s">
         <v>101</v>
       </c>
@@ -5811,11 +6261,15 @@
       <c r="H62" s="14">
         <v>0.1</v>
       </c>
-      <c r="I62" s="14"/>
+      <c r="I62" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J62" s="14">
         <v>8.1</v>
       </c>
-      <c r="K62" s="14"/>
+      <c r="K62" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L62" s="12" t="s">
         <v>102</v>
       </c>
@@ -5863,11 +6317,15 @@
       <c r="H63" s="14">
         <v>0.1</v>
       </c>
-      <c r="I63" s="14"/>
+      <c r="I63" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J63" s="14">
         <v>8.1</v>
       </c>
-      <c r="K63" s="14"/>
+      <c r="K63" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L63" s="12" t="s">
         <v>103</v>
       </c>
@@ -5915,11 +6373,15 @@
       <c r="H64" s="14">
         <v>0.1</v>
       </c>
-      <c r="I64" s="14"/>
+      <c r="I64" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J64" s="14">
         <v>8.1</v>
       </c>
-      <c r="K64" s="14"/>
+      <c r="K64" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L64" s="12" t="s">
         <v>104</v>
       </c>
@@ -5967,11 +6429,15 @@
       <c r="H65" s="14">
         <v>0.1</v>
       </c>
-      <c r="I65" s="14"/>
+      <c r="I65" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J65" s="14">
         <v>8.1</v>
       </c>
-      <c r="K65" s="14"/>
+      <c r="K65" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L65" s="12" t="s">
         <v>105</v>
       </c>
@@ -6019,11 +6485,15 @@
       <c r="H66" s="14">
         <v>0.1</v>
       </c>
-      <c r="I66" s="14"/>
+      <c r="I66" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J66" s="14">
         <v>8.1</v>
       </c>
-      <c r="K66" s="14"/>
+      <c r="K66" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L66" s="12" t="s">
         <v>106</v>
       </c>
@@ -6071,11 +6541,15 @@
       <c r="H67" s="14">
         <v>0.1</v>
       </c>
-      <c r="I67" s="14"/>
+      <c r="I67" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J67" s="14">
         <v>8.1</v>
       </c>
-      <c r="K67" s="14"/>
+      <c r="K67" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L67" s="12" t="s">
         <v>107</v>
       </c>
@@ -6123,11 +6597,15 @@
       <c r="H68" s="14">
         <v>0.3</v>
       </c>
-      <c r="I68" s="14"/>
+      <c r="I68" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J68" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K68" s="14"/>
+      <c r="K68" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L68" s="12" t="s">
         <v>108</v>
       </c>
@@ -6175,11 +6653,15 @@
       <c r="H69" s="14">
         <v>0.3</v>
       </c>
-      <c r="I69" s="14"/>
+      <c r="I69" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J69" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K69" s="14"/>
+      <c r="K69" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L69" s="12" t="s">
         <v>109</v>
       </c>
@@ -6227,11 +6709,15 @@
       <c r="H70" s="14">
         <v>0.3</v>
       </c>
-      <c r="I70" s="14"/>
+      <c r="I70" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J70" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K70" s="14"/>
+      <c r="K70" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L70" s="12" t="s">
         <v>110</v>
       </c>
@@ -6279,11 +6765,15 @@
       <c r="H71" s="14">
         <v>0.3</v>
       </c>
-      <c r="I71" s="14"/>
+      <c r="I71" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J71" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K71" s="14"/>
+      <c r="K71" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L71" s="12" t="s">
         <v>111</v>
       </c>
@@ -6331,11 +6821,15 @@
       <c r="H72" s="14">
         <v>0.2</v>
       </c>
-      <c r="I72" s="14"/>
+      <c r="I72" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J72" s="14">
         <v>8</v>
       </c>
-      <c r="K72" s="14"/>
+      <c r="K72" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L72" s="12" t="s">
         <v>112</v>
       </c>
@@ -6383,11 +6877,15 @@
       <c r="H73" s="14">
         <v>0.2</v>
       </c>
-      <c r="I73" s="14"/>
+      <c r="I73" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J73" s="14">
         <v>8</v>
       </c>
-      <c r="K73" s="14"/>
+      <c r="K73" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L73" s="12" t="s">
         <v>113</v>
       </c>
@@ -6435,11 +6933,15 @@
       <c r="H74" s="14">
         <v>0.2</v>
       </c>
-      <c r="I74" s="14"/>
+      <c r="I74" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J74" s="14">
         <v>8</v>
       </c>
-      <c r="K74" s="14"/>
+      <c r="K74" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L74" s="12" t="s">
         <v>114</v>
       </c>
@@ -6487,11 +6989,15 @@
       <c r="H75" s="14">
         <v>0.5</v>
       </c>
-      <c r="I75" s="14"/>
+      <c r="I75" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J75" s="14">
         <v>14.2</v>
       </c>
-      <c r="K75" s="14"/>
+      <c r="K75" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L75" s="12" t="s">
         <v>115</v>
       </c>
@@ -6539,11 +7045,15 @@
       <c r="H76" s="14">
         <v>0.5</v>
       </c>
-      <c r="I76" s="14"/>
+      <c r="I76" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J76" s="14">
         <v>14.2</v>
       </c>
-      <c r="K76" s="14"/>
+      <c r="K76" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L76" s="12" t="s">
         <v>116</v>
       </c>
@@ -6591,11 +7101,15 @@
       <c r="H77" s="14">
         <v>0.5</v>
       </c>
-      <c r="I77" s="14"/>
+      <c r="I77" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J77" s="14">
         <v>14.2</v>
       </c>
-      <c r="K77" s="14"/>
+      <c r="K77" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L77" s="12" t="s">
         <v>117</v>
       </c>
@@ -6643,11 +7157,15 @@
       <c r="H78" s="14">
         <v>0.5</v>
       </c>
-      <c r="I78" s="14"/>
+      <c r="I78" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J78" s="14">
         <v>14.2</v>
       </c>
-      <c r="K78" s="14"/>
+      <c r="K78" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L78" s="12" t="s">
         <v>118</v>
       </c>
@@ -6695,11 +7213,15 @@
       <c r="H79" s="14">
         <v>0.5</v>
       </c>
-      <c r="I79" s="14"/>
+      <c r="I79" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J79" s="14">
         <v>14.2</v>
       </c>
-      <c r="K79" s="14"/>
+      <c r="K79" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L79" s="12" t="s">
         <v>119</v>
       </c>
@@ -6747,11 +7269,15 @@
       <c r="H80" s="14">
         <v>0.5</v>
       </c>
-      <c r="I80" s="14"/>
+      <c r="I80" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J80" s="14">
         <v>14.2</v>
       </c>
-      <c r="K80" s="14"/>
+      <c r="K80" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L80" s="12" t="s">
         <v>120</v>
       </c>
@@ -6799,11 +7325,15 @@
       <c r="H81" s="14">
         <v>0.5</v>
       </c>
-      <c r="I81" s="14"/>
+      <c r="I81" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J81" s="14">
         <v>14.2</v>
       </c>
-      <c r="K81" s="14"/>
+      <c r="K81" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L81" s="12" t="s">
         <v>121</v>
       </c>
@@ -6851,11 +7381,15 @@
       <c r="H82" s="14">
         <v>0.5</v>
       </c>
-      <c r="I82" s="14"/>
+      <c r="I82" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J82" s="14">
         <v>12.6</v>
       </c>
-      <c r="K82" s="14"/>
+      <c r="K82" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L82" s="12" t="s">
         <v>122</v>
       </c>
@@ -6903,11 +7437,15 @@
       <c r="H83" s="14">
         <v>0.5</v>
       </c>
-      <c r="I83" s="14"/>
+      <c r="I83" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J83" s="14">
         <v>12.6</v>
       </c>
-      <c r="K83" s="14"/>
+      <c r="K83" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L83" s="12" t="s">
         <v>123</v>
       </c>
@@ -6955,11 +7493,15 @@
       <c r="H84" s="14">
         <v>0.5</v>
       </c>
-      <c r="I84" s="14"/>
+      <c r="I84" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J84" s="14">
         <v>12.6</v>
       </c>
-      <c r="K84" s="14"/>
+      <c r="K84" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L84" s="12" t="s">
         <v>124</v>
       </c>
@@ -7007,11 +7549,15 @@
       <c r="H85" s="14">
         <v>0.5</v>
       </c>
-      <c r="I85" s="14"/>
+      <c r="I85" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J85" s="14">
         <v>12.6</v>
       </c>
-      <c r="K85" s="14"/>
+      <c r="K85" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L85" s="12" t="s">
         <v>125</v>
       </c>
@@ -7059,11 +7605,15 @@
       <c r="H86" s="14">
         <v>0.5</v>
       </c>
-      <c r="I86" s="14"/>
+      <c r="I86" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J86" s="14">
         <v>12.6</v>
       </c>
-      <c r="K86" s="14"/>
+      <c r="K86" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L86" s="12" t="s">
         <v>126</v>
       </c>
@@ -7111,11 +7661,15 @@
       <c r="H87" s="14">
         <v>0.7</v>
       </c>
-      <c r="I87" s="14"/>
+      <c r="I87" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J87" s="14">
         <v>11.2</v>
       </c>
-      <c r="K87" s="14"/>
+      <c r="K87" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L87" s="12" t="s">
         <v>127</v>
       </c>
@@ -7163,11 +7717,15 @@
       <c r="H88" s="14">
         <v>0.7</v>
       </c>
-      <c r="I88" s="14"/>
+      <c r="I88" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J88" s="14">
         <v>11.2</v>
       </c>
-      <c r="K88" s="14"/>
+      <c r="K88" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L88" s="12" t="s">
         <v>128</v>
       </c>
@@ -7215,11 +7773,15 @@
       <c r="H89" s="14">
         <v>0.7</v>
       </c>
-      <c r="I89" s="14"/>
+      <c r="I89" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J89" s="14">
         <v>11.2</v>
       </c>
-      <c r="K89" s="14"/>
+      <c r="K89" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L89" s="12" t="s">
         <v>129</v>
       </c>
@@ -7267,11 +7829,15 @@
       <c r="H90" s="14">
         <v>0.7</v>
       </c>
-      <c r="I90" s="14"/>
+      <c r="I90" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J90" s="14">
         <v>11.2</v>
       </c>
-      <c r="K90" s="14"/>
+      <c r="K90" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L90" s="12" t="s">
         <v>130</v>
       </c>
@@ -7319,11 +7885,15 @@
       <c r="H91" s="14">
         <v>0.7</v>
       </c>
-      <c r="I91" s="14"/>
+      <c r="I91" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J91" s="14">
         <v>11.2</v>
       </c>
-      <c r="K91" s="14"/>
+      <c r="K91" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L91" s="12" t="s">
         <v>131</v>
       </c>
@@ -7371,11 +7941,15 @@
       <c r="H92" s="14">
         <v>0.4</v>
       </c>
-      <c r="I92" s="14"/>
+      <c r="I92" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J92" s="14">
         <v>18</v>
       </c>
-      <c r="K92" s="14"/>
+      <c r="K92" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L92" s="12" t="s">
         <v>132</v>
       </c>
@@ -7423,11 +7997,15 @@
       <c r="H93" s="14">
         <v>0.4</v>
       </c>
-      <c r="I93" s="14"/>
+      <c r="I93" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J93" s="14">
         <v>18</v>
       </c>
-      <c r="K93" s="14"/>
+      <c r="K93" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L93" s="12" t="s">
         <v>133</v>
       </c>
@@ -7475,11 +8053,15 @@
       <c r="H94" s="14">
         <v>0.4</v>
       </c>
-      <c r="I94" s="14"/>
+      <c r="I94" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J94" s="14">
         <v>18</v>
       </c>
-      <c r="K94" s="14"/>
+      <c r="K94" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L94" s="12" t="s">
         <v>134</v>
       </c>
@@ -7527,11 +8109,15 @@
       <c r="H95" s="14">
         <v>0.4</v>
       </c>
-      <c r="I95" s="14"/>
+      <c r="I95" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J95" s="14">
         <v>18</v>
       </c>
-      <c r="K95" s="14"/>
+      <c r="K95" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L95" s="12" t="s">
         <v>135</v>
       </c>
@@ -7579,11 +8165,15 @@
       <c r="H96" s="14">
         <v>0.4</v>
       </c>
-      <c r="I96" s="14"/>
+      <c r="I96" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J96" s="14">
         <v>18</v>
       </c>
-      <c r="K96" s="14"/>
+      <c r="K96" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L96" s="12" t="s">
         <v>136</v>
       </c>
@@ -7631,11 +8221,15 @@
       <c r="H97" s="14">
         <v>0.4</v>
       </c>
-      <c r="I97" s="14"/>
+      <c r="I97" s="14" t="s">
+        <v>396</v>
+      </c>
       <c r="J97" s="14">
         <v>18</v>
       </c>
-      <c r="K97" s="14"/>
+      <c r="K97" s="20">
+        <v>12.3</v>
+      </c>
       <c r="L97" s="12" t="s">
         <v>137</v>
       </c>
@@ -7683,15 +8277,21 @@
       <c r="H98" s="14">
         <v>0</v>
       </c>
-      <c r="I98" s="14"/>
+      <c r="I98" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="J98" s="14">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K98" s="14"/>
+      <c r="K98" s="20">
+        <v>108</v>
+      </c>
       <c r="L98" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="M98" s="16"/>
+      <c r="M98" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="N98" s="48">
         <v>69</v>
       </c>
@@ -7733,11 +8333,15 @@
       <c r="H99" s="14">
         <v>0.2</v>
       </c>
-      <c r="I99" s="14"/>
+      <c r="I99" s="14" t="s">
+        <v>397</v>
+      </c>
       <c r="J99" s="14">
         <v>5.9</v>
       </c>
-      <c r="K99" s="14"/>
+      <c r="K99" s="20">
+        <v>108</v>
+      </c>
       <c r="L99" s="12" t="s">
         <v>140</v>
       </c>
@@ -7785,11 +8389,15 @@
       <c r="H100" s="14">
         <v>0</v>
       </c>
-      <c r="I100" s="14"/>
+      <c r="I100" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J100" s="14">
         <v>7.8</v>
       </c>
-      <c r="K100" s="14"/>
+      <c r="K100" s="20">
+        <v>108</v>
+      </c>
       <c r="L100" s="12" t="s">
         <v>141</v>
       </c>
@@ -7837,11 +8445,15 @@
       <c r="H101" s="14">
         <v>0</v>
       </c>
-      <c r="I101" s="14"/>
+      <c r="I101" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J101" s="14">
         <v>7.8</v>
       </c>
-      <c r="K101" s="14"/>
+      <c r="K101" s="20">
+        <v>108</v>
+      </c>
       <c r="L101" s="12" t="s">
         <v>142</v>
       </c>
@@ -7889,11 +8501,15 @@
       <c r="H102" s="14">
         <v>0</v>
       </c>
-      <c r="I102" s="14"/>
+      <c r="I102" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J102" s="14">
         <v>7.8</v>
       </c>
-      <c r="K102" s="14"/>
+      <c r="K102" s="20">
+        <v>108</v>
+      </c>
       <c r="L102" s="12" t="s">
         <v>143</v>
       </c>
@@ -7941,11 +8557,15 @@
       <c r="H103" s="14">
         <v>0</v>
       </c>
-      <c r="I103" s="14"/>
+      <c r="I103" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J103" s="14">
         <v>7.1</v>
       </c>
-      <c r="K103" s="14"/>
+      <c r="K103" s="20">
+        <v>108</v>
+      </c>
       <c r="L103" s="12" t="s">
         <v>144</v>
       </c>
@@ -7993,11 +8613,15 @@
       <c r="H104" s="14">
         <v>0</v>
       </c>
-      <c r="I104" s="14"/>
+      <c r="I104" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J104" s="14">
         <v>7.1</v>
       </c>
-      <c r="K104" s="14"/>
+      <c r="K104" s="20">
+        <v>108</v>
+      </c>
       <c r="L104" s="12" t="s">
         <v>145</v>
       </c>
@@ -8045,11 +8669,15 @@
       <c r="H105" s="14">
         <v>0</v>
       </c>
-      <c r="I105" s="14"/>
+      <c r="I105" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J105" s="14">
         <v>7.1</v>
       </c>
-      <c r="K105" s="14"/>
+      <c r="K105" s="20">
+        <v>108</v>
+      </c>
       <c r="L105" s="12" t="s">
         <v>146</v>
       </c>
@@ -8097,11 +8725,15 @@
       <c r="H106" s="14">
         <v>0</v>
       </c>
-      <c r="I106" s="14"/>
+      <c r="I106" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J106" s="14">
         <v>11.8</v>
       </c>
-      <c r="K106" s="14"/>
+      <c r="K106" s="20">
+        <v>108</v>
+      </c>
       <c r="L106" s="12" t="s">
         <v>147</v>
       </c>
@@ -8149,11 +8781,15 @@
       <c r="H107" s="14">
         <v>0</v>
       </c>
-      <c r="I107" s="14"/>
+      <c r="I107" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J107" s="14">
         <v>11.8</v>
       </c>
-      <c r="K107" s="14"/>
+      <c r="K107" s="20">
+        <v>108</v>
+      </c>
       <c r="L107" s="12" t="s">
         <v>148</v>
       </c>
@@ -8201,11 +8837,15 @@
       <c r="H108" s="14">
         <v>0</v>
       </c>
-      <c r="I108" s="14"/>
+      <c r="I108" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J108" s="14">
         <v>11.8</v>
       </c>
-      <c r="K108" s="14"/>
+      <c r="K108" s="20">
+        <v>108</v>
+      </c>
       <c r="L108" s="12" t="s">
         <v>149</v>
       </c>
@@ -8253,11 +8893,15 @@
       <c r="H109" s="14">
         <v>0.2</v>
       </c>
-      <c r="I109" s="14"/>
+      <c r="I109" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J109" s="14">
         <v>8.1</v>
       </c>
-      <c r="K109" s="14"/>
+      <c r="K109" s="20">
+        <v>108</v>
+      </c>
       <c r="L109" s="12" t="s">
         <v>203</v>
       </c>
@@ -8305,11 +8949,15 @@
       <c r="H110" s="14">
         <v>0.2</v>
       </c>
-      <c r="I110" s="14"/>
+      <c r="I110" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J110" s="14">
         <v>8.1</v>
       </c>
-      <c r="K110" s="14"/>
+      <c r="K110" s="20">
+        <v>108</v>
+      </c>
       <c r="L110" s="12" t="s">
         <v>150</v>
       </c>
@@ -8357,11 +9005,15 @@
       <c r="H111" s="14">
         <v>0.2</v>
       </c>
-      <c r="I111" s="14"/>
+      <c r="I111" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J111" s="14">
         <v>8.1</v>
       </c>
-      <c r="K111" s="14"/>
+      <c r="K111" s="20">
+        <v>108</v>
+      </c>
       <c r="L111" s="12" t="s">
         <v>151</v>
       </c>
@@ -8409,11 +9061,15 @@
       <c r="H112" s="14">
         <v>0.5</v>
       </c>
-      <c r="I112" s="14"/>
+      <c r="I112" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J112" s="14">
         <v>4.3</v>
       </c>
-      <c r="K112" s="14"/>
+      <c r="K112" s="20">
+        <v>108</v>
+      </c>
       <c r="L112" s="12" t="s">
         <v>153</v>
       </c>
@@ -8461,11 +9117,15 @@
       <c r="H113" s="14">
         <v>0.5</v>
       </c>
-      <c r="I113" s="14"/>
+      <c r="I113" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J113" s="14">
         <v>4.3</v>
       </c>
-      <c r="K113" s="14"/>
+      <c r="K113" s="20">
+        <v>108</v>
+      </c>
       <c r="L113" s="12" t="s">
         <v>154</v>
       </c>
@@ -8513,11 +9173,15 @@
       <c r="H114" s="14">
         <v>0.5</v>
       </c>
-      <c r="I114" s="14"/>
+      <c r="I114" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J114" s="14">
         <v>5.0999999999999996</v>
       </c>
-      <c r="K114" s="14"/>
+      <c r="K114" s="20">
+        <v>108</v>
+      </c>
       <c r="L114" s="12" t="s">
         <v>155</v>
       </c>
@@ -8565,11 +9229,15 @@
       <c r="H115" s="14">
         <v>0.5</v>
       </c>
-      <c r="I115" s="14"/>
+      <c r="I115" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J115" s="14">
         <v>5.0999999999999996</v>
       </c>
-      <c r="K115" s="14"/>
+      <c r="K115" s="20">
+        <v>108</v>
+      </c>
       <c r="L115" s="12" t="s">
         <v>156</v>
       </c>
@@ -8617,11 +9285,15 @@
       <c r="H116" s="14">
         <v>0.7</v>
       </c>
-      <c r="I116" s="14"/>
+      <c r="I116" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J116" s="14">
         <v>3.7</v>
       </c>
-      <c r="K116" s="14"/>
+      <c r="K116" s="20">
+        <v>108</v>
+      </c>
       <c r="L116" s="12" t="s">
         <v>157</v>
       </c>
@@ -8669,11 +9341,15 @@
       <c r="H117" s="14">
         <v>0.7</v>
       </c>
-      <c r="I117" s="14"/>
+      <c r="I117" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J117" s="14">
         <v>3.7</v>
       </c>
-      <c r="K117" s="14"/>
+      <c r="K117" s="20">
+        <v>108</v>
+      </c>
       <c r="L117" s="12" t="s">
         <v>158</v>
       </c>
@@ -8721,11 +9397,15 @@
       <c r="H118" s="14">
         <v>0.6</v>
       </c>
-      <c r="I118" s="14"/>
+      <c r="I118" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J118" s="14">
         <v>7.5</v>
       </c>
-      <c r="K118" s="14"/>
+      <c r="K118" s="20">
+        <v>108</v>
+      </c>
       <c r="L118" s="12" t="s">
         <v>159</v>
       </c>
@@ -8773,11 +9453,15 @@
       <c r="H119" s="14">
         <v>0.6</v>
       </c>
-      <c r="I119" s="14"/>
+      <c r="I119" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J119" s="14">
         <v>7.5</v>
       </c>
-      <c r="K119" s="14"/>
+      <c r="K119" s="20">
+        <v>108</v>
+      </c>
       <c r="L119" s="12" t="s">
         <v>160</v>
       </c>
@@ -8825,11 +9509,15 @@
       <c r="H120" s="14">
         <v>0.7</v>
       </c>
-      <c r="I120" s="14"/>
+      <c r="I120" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J120" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K120" s="14"/>
+      <c r="K120" s="20">
+        <v>108</v>
+      </c>
       <c r="L120" s="12" t="s">
         <v>161</v>
       </c>
@@ -8877,11 +9565,15 @@
       <c r="H121" s="14">
         <v>0.7</v>
       </c>
-      <c r="I121" s="14"/>
+      <c r="I121" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J121" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K121" s="14"/>
+      <c r="K121" s="20">
+        <v>108</v>
+      </c>
       <c r="L121" s="12" t="s">
         <v>162</v>
       </c>
@@ -8929,11 +9621,15 @@
       <c r="H122" s="14">
         <v>0.7</v>
       </c>
-      <c r="I122" s="14"/>
+      <c r="I122" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J122" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K122" s="14"/>
+      <c r="K122" s="20">
+        <v>108</v>
+      </c>
       <c r="L122" s="12" t="s">
         <v>163</v>
       </c>
@@ -8981,11 +9677,15 @@
       <c r="H123" s="14">
         <v>0.8</v>
       </c>
-      <c r="I123" s="14"/>
+      <c r="I123" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J123" s="14">
         <v>6.8</v>
       </c>
-      <c r="K123" s="14"/>
+      <c r="K123" s="20">
+        <v>108</v>
+      </c>
       <c r="L123" s="12" t="s">
         <v>164</v>
       </c>
@@ -9033,11 +9733,15 @@
       <c r="H124" s="14">
         <v>0.8</v>
       </c>
-      <c r="I124" s="14"/>
+      <c r="I124" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J124" s="14">
         <v>6.8</v>
       </c>
-      <c r="K124" s="14"/>
+      <c r="K124" s="20">
+        <v>108</v>
+      </c>
       <c r="L124" s="12" t="s">
         <v>165</v>
       </c>
@@ -9085,11 +9789,15 @@
       <c r="H125" s="14">
         <v>0</v>
       </c>
-      <c r="I125" s="14"/>
+      <c r="I125" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J125" s="14">
         <v>7.3</v>
       </c>
-      <c r="K125" s="14"/>
+      <c r="K125" s="20">
+        <v>2.17</v>
+      </c>
       <c r="L125" s="12" t="s">
         <v>167</v>
       </c>
@@ -9137,11 +9845,15 @@
       <c r="H126" s="14">
         <v>0</v>
       </c>
-      <c r="I126" s="14"/>
+      <c r="I126" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J126" s="14">
         <v>7.3</v>
       </c>
-      <c r="K126" s="14"/>
+      <c r="K126" s="20">
+        <v>2.17</v>
+      </c>
       <c r="L126" s="12" t="s">
         <v>168</v>
       </c>
@@ -9189,11 +9901,15 @@
       <c r="H127" s="14">
         <v>0.1</v>
       </c>
-      <c r="I127" s="14"/>
+      <c r="I127" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J127" s="14">
         <v>5.9</v>
       </c>
-      <c r="K127" s="14"/>
+      <c r="K127" s="20">
+        <v>2.17</v>
+      </c>
       <c r="L127" s="12" t="s">
         <v>169</v>
       </c>
@@ -9241,11 +9957,15 @@
       <c r="H128" s="14">
         <v>0.1</v>
       </c>
-      <c r="I128" s="14"/>
+      <c r="I128" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J128" s="14">
         <v>5.9</v>
       </c>
-      <c r="K128" s="14"/>
+      <c r="K128" s="20">
+        <v>2.17</v>
+      </c>
       <c r="L128" s="12" t="s">
         <v>170</v>
       </c>
@@ -9293,11 +10013,15 @@
       <c r="H129" s="14">
         <v>0.3</v>
       </c>
-      <c r="I129" s="14"/>
+      <c r="I129" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J129" s="14">
         <v>4.8</v>
       </c>
-      <c r="K129" s="14"/>
+      <c r="K129" s="20">
+        <v>2.17</v>
+      </c>
       <c r="L129" s="12" t="s">
         <v>171</v>
       </c>
@@ -9345,11 +10069,15 @@
       <c r="H130" s="14">
         <v>0.3</v>
       </c>
-      <c r="I130" s="14"/>
+      <c r="I130" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J130" s="14">
         <v>4.8</v>
       </c>
-      <c r="K130" s="14"/>
+      <c r="K130" s="20">
+        <v>2.17</v>
+      </c>
       <c r="L130" s="12" t="s">
         <v>172</v>
       </c>
@@ -9397,11 +10125,15 @@
       <c r="H131" s="14">
         <v>0</v>
       </c>
-      <c r="I131" s="14"/>
+      <c r="I131" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="J131" s="14">
         <v>7.3</v>
       </c>
-      <c r="K131" s="14"/>
+      <c r="K131" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L131" s="12" t="s">
         <v>174</v>
       </c>
@@ -9449,11 +10181,15 @@
       <c r="H132" s="14">
         <v>0.1</v>
       </c>
-      <c r="I132" s="14"/>
+      <c r="I132" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J132" s="14">
         <v>8.4</v>
       </c>
-      <c r="K132" s="14"/>
+      <c r="K132" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L132" s="12" t="s">
         <v>175</v>
       </c>
@@ -9501,11 +10237,15 @@
       <c r="H133" s="14">
         <v>0.1</v>
       </c>
-      <c r="I133" s="14"/>
+      <c r="I133" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J133" s="14">
         <v>8.4</v>
       </c>
-      <c r="K133" s="14"/>
+      <c r="K133" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L133" s="12" t="s">
         <v>176</v>
       </c>
@@ -9553,11 +10293,15 @@
       <c r="H134" s="14">
         <v>0.1</v>
       </c>
-      <c r="I134" s="14"/>
+      <c r="I134" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J134" s="14">
         <v>8.4</v>
       </c>
-      <c r="K134" s="14"/>
+      <c r="K134" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L134" s="12" t="s">
         <v>177</v>
       </c>
@@ -9605,11 +10349,15 @@
       <c r="H135" s="14">
         <v>0.1</v>
       </c>
-      <c r="I135" s="14"/>
+      <c r="I135" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J135" s="14">
         <v>8.4</v>
       </c>
-      <c r="K135" s="14"/>
+      <c r="K135" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L135" s="12" t="s">
         <v>178</v>
       </c>
@@ -9657,11 +10405,15 @@
       <c r="H136" s="14">
         <v>0.1</v>
       </c>
-      <c r="I136" s="14"/>
+      <c r="I136" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="J136" s="14">
         <v>8.4</v>
       </c>
-      <c r="K136" s="14"/>
+      <c r="K136" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L136" s="12" t="s">
         <v>179</v>
       </c>
@@ -9709,11 +10461,15 @@
       <c r="H137" s="14">
         <v>0.2</v>
       </c>
-      <c r="I137" s="14"/>
+      <c r="I137" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J137" s="14">
         <v>6.5</v>
       </c>
-      <c r="K137" s="14"/>
+      <c r="K137" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L137" s="12" t="s">
         <v>180</v>
       </c>
@@ -9761,11 +10517,15 @@
       <c r="H138" s="14">
         <v>0.2</v>
       </c>
-      <c r="I138" s="14"/>
+      <c r="I138" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J138" s="14">
         <v>6.5</v>
       </c>
-      <c r="K138" s="14"/>
+      <c r="K138" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L138" s="12" t="s">
         <v>181</v>
       </c>
@@ -9813,11 +10573,15 @@
       <c r="H139" s="14">
         <v>0.2</v>
       </c>
-      <c r="I139" s="14"/>
+      <c r="I139" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J139" s="14">
         <v>9.4</v>
       </c>
-      <c r="K139" s="14"/>
+      <c r="K139" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L139" s="12" t="s">
         <v>182</v>
       </c>
@@ -9865,11 +10629,15 @@
       <c r="H140" s="14">
         <v>0.2</v>
       </c>
-      <c r="I140" s="14"/>
+      <c r="I140" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J140" s="14">
         <v>9.4</v>
       </c>
-      <c r="K140" s="14"/>
+      <c r="K140" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L140" s="12" t="s">
         <v>183</v>
       </c>
@@ -9917,11 +10685,15 @@
       <c r="H141" s="14">
         <v>0.2</v>
       </c>
-      <c r="I141" s="14"/>
+      <c r="I141" s="14" t="s">
+        <v>395</v>
+      </c>
       <c r="J141" s="14">
         <v>9.4</v>
       </c>
-      <c r="K141" s="14"/>
+      <c r="K141" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L141" s="12" t="s">
         <v>184</v>
       </c>
@@ -9969,11 +10741,15 @@
       <c r="H142" s="14">
         <v>0.2</v>
       </c>
-      <c r="I142" s="14"/>
+      <c r="I142" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J142" s="14">
         <v>5.3</v>
       </c>
-      <c r="K142" s="14"/>
+      <c r="K142" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L142" s="12" t="s">
         <v>185</v>
       </c>
@@ -10021,11 +10797,15 @@
       <c r="H143" s="14">
         <v>0.2</v>
       </c>
-      <c r="I143" s="14"/>
+      <c r="I143" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J143" s="14">
         <v>5.3</v>
       </c>
-      <c r="K143" s="14"/>
+      <c r="K143" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L143" s="12" t="s">
         <v>186</v>
       </c>
@@ -10073,11 +10853,15 @@
       <c r="H144" s="14">
         <v>0.2</v>
       </c>
-      <c r="I144" s="14"/>
+      <c r="I144" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="J144" s="14">
         <v>7.6</v>
       </c>
-      <c r="K144" s="14"/>
+      <c r="K144" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L144" s="12" t="s">
         <v>187</v>
       </c>
@@ -10125,11 +10909,15 @@
       <c r="H145" s="14">
         <v>0.5</v>
       </c>
-      <c r="I145" s="14"/>
+      <c r="I145" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J145" s="14">
         <v>3.5</v>
       </c>
-      <c r="K145" s="14"/>
+      <c r="K145" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L145" s="12" t="s">
         <v>188</v>
       </c>
@@ -10177,11 +10965,15 @@
       <c r="H146" s="14">
         <v>0.5</v>
       </c>
-      <c r="I146" s="14"/>
+      <c r="I146" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J146" s="14">
         <v>6.4</v>
       </c>
-      <c r="K146" s="14"/>
+      <c r="K146" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L146" s="12" t="s">
         <v>189</v>
       </c>
@@ -10229,11 +11021,15 @@
       <c r="H147" s="14">
         <v>0.6</v>
       </c>
-      <c r="I147" s="14"/>
+      <c r="I147" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J147" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K147" s="14"/>
+      <c r="K147" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L147" s="12" t="s">
         <v>190</v>
       </c>
@@ -10281,11 +11077,15 @@
       <c r="H148" s="14">
         <v>0.6</v>
       </c>
-      <c r="I148" s="14"/>
+      <c r="I148" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J148" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K148" s="14"/>
+      <c r="K148" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L148" s="12" t="s">
         <v>191</v>
       </c>
@@ -10333,11 +11133,15 @@
       <c r="H149" s="14">
         <v>0.6</v>
       </c>
-      <c r="I149" s="14"/>
+      <c r="I149" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J149" s="14">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K149" s="14"/>
+      <c r="K149" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L149" s="12" t="s">
         <v>192</v>
       </c>
@@ -10385,11 +11189,15 @@
       <c r="H150" s="14">
         <v>0.7</v>
       </c>
-      <c r="I150" s="14"/>
+      <c r="I150" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J150" s="14">
         <v>3.6</v>
       </c>
-      <c r="K150" s="14"/>
+      <c r="K150" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L150" s="12" t="s">
         <v>193</v>
       </c>
@@ -10438,11 +11246,15 @@
       <c r="H151" s="14">
         <v>0.7</v>
       </c>
-      <c r="I151" s="14"/>
+      <c r="I151" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="J151" s="14">
         <v>3.6</v>
       </c>
-      <c r="K151" s="14"/>
+      <c r="K151" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L151" s="12" t="s">
         <v>194</v>
       </c>
@@ -10491,11 +11303,15 @@
       <c r="H152" s="14">
         <v>0.4</v>
       </c>
-      <c r="I152" s="14"/>
+      <c r="I152" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="J152" s="14">
         <v>9.4</v>
       </c>
-      <c r="K152" s="14"/>
+      <c r="K152" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L152" s="12" t="s">
         <v>195</v>
       </c>
@@ -10544,11 +11360,15 @@
       <c r="H153" s="14">
         <v>0.4</v>
       </c>
-      <c r="I153" s="14"/>
+      <c r="I153" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="J153" s="14">
         <v>9.4</v>
       </c>
-      <c r="K153" s="14"/>
+      <c r="K153" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L153" s="12" t="s">
         <v>196</v>
       </c>
@@ -10597,11 +11417,15 @@
       <c r="H154" s="30">
         <v>0.4</v>
       </c>
-      <c r="I154" s="30"/>
+      <c r="I154" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="J154" s="30">
         <v>9.4</v>
       </c>
-      <c r="K154" s="30"/>
+      <c r="K154" s="20">
+        <v>44.4</v>
+      </c>
       <c r="L154" s="29" t="s">
         <v>197</v>
       </c>
@@ -10653,7 +11477,9 @@
       <c r="I155" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="J155" s="25"/>
+      <c r="J155" s="25">
+        <v>4</v>
+      </c>
       <c r="K155" s="27">
         <v>1282</v>
       </c>
@@ -10705,7 +11531,9 @@
       <c r="I156" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J156" s="14"/>
+      <c r="J156" s="14">
+        <v>4</v>
+      </c>
       <c r="K156" s="20">
         <v>1282</v>
       </c>
@@ -10757,7 +11585,9 @@
       <c r="I157" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J157" s="14"/>
+      <c r="J157" s="14">
+        <v>4.7</v>
+      </c>
       <c r="K157" s="20">
         <v>1282</v>
       </c>
@@ -10809,7 +11639,9 @@
       <c r="I158" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J158" s="14"/>
+      <c r="J158" s="14">
+        <v>4.7</v>
+      </c>
       <c r="K158" s="20">
         <v>1282</v>
       </c>
@@ -10861,7 +11693,9 @@
       <c r="I159" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="J159" s="14"/>
+      <c r="J159" s="14">
+        <v>10.199999999999999</v>
+      </c>
       <c r="K159" s="20">
         <v>1282</v>
       </c>
@@ -10914,7 +11748,9 @@
       <c r="I160" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="J160" s="14"/>
+      <c r="J160" s="14">
+        <v>10.199999999999999</v>
+      </c>
       <c r="K160" s="20">
         <v>1282</v>
       </c>
@@ -10966,7 +11802,9 @@
       <c r="I161" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J161" s="14"/>
+      <c r="J161" s="14">
+        <v>12.1</v>
+      </c>
       <c r="K161" s="20">
         <v>2.1800000000000002</v>
       </c>
@@ -11018,7 +11856,9 @@
       <c r="I162" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J162" s="14"/>
+      <c r="J162" s="14">
+        <v>12.1</v>
+      </c>
       <c r="K162" s="20">
         <v>2.1800000000000002</v>
       </c>
@@ -11070,7 +11910,9 @@
       <c r="I163" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J163" s="14"/>
+      <c r="J163" s="14">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="K163" s="20">
         <v>2.1800000000000002</v>
       </c>
@@ -11122,7 +11964,9 @@
       <c r="I164" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J164" s="14"/>
+      <c r="J164" s="14">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="K164" s="20">
         <v>2.1800000000000002</v>
       </c>
@@ -11174,7 +12018,9 @@
       <c r="I165" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="J165" s="14"/>
+      <c r="J165" s="14">
+        <v>7.7</v>
+      </c>
       <c r="K165" s="20">
         <v>2.1800000000000002</v>
       </c>
@@ -11226,7 +12072,9 @@
       <c r="I166" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="J166" s="14"/>
+      <c r="J166" s="14">
+        <v>7.7</v>
+      </c>
       <c r="K166" s="20">
         <v>2.1800000000000002</v>
       </c>
@@ -11278,7 +12126,9 @@
       <c r="I167" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J167" s="14"/>
+      <c r="J167" s="14">
+        <v>6.2</v>
+      </c>
       <c r="K167" s="20">
         <v>1282</v>
       </c>
@@ -11330,7 +12180,9 @@
       <c r="I168" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J168" s="14"/>
+      <c r="J168" s="14">
+        <v>6.2</v>
+      </c>
       <c r="K168" s="20">
         <v>1282</v>
       </c>
@@ -11382,7 +12234,9 @@
       <c r="I169" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J169" s="14"/>
+      <c r="J169" s="14">
+        <v>3.6</v>
+      </c>
       <c r="K169" s="20">
         <v>1282</v>
       </c>
@@ -11434,7 +12288,9 @@
       <c r="I170" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J170" s="14"/>
+      <c r="J170" s="14">
+        <v>5.7</v>
+      </c>
       <c r="K170" s="20">
         <v>1282</v>
       </c>
@@ -11486,7 +12342,9 @@
       <c r="I171" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="J171" s="14"/>
+      <c r="J171" s="14">
+        <v>4.0999999999999996</v>
+      </c>
       <c r="K171" s="20">
         <v>1282</v>
       </c>
@@ -11539,7 +12397,9 @@
       <c r="I172" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="J172" s="14"/>
+      <c r="J172" s="14">
+        <v>4.8</v>
+      </c>
       <c r="K172" s="20">
         <v>1282</v>
       </c>
@@ -11591,7 +12451,9 @@
       <c r="I173" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="J173" s="14"/>
+      <c r="J173" s="14">
+        <v>9</v>
+      </c>
       <c r="K173" s="20">
         <v>73.3</v>
       </c>
@@ -11643,7 +12505,9 @@
       <c r="I174" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="J174" s="14"/>
+      <c r="J174" s="14">
+        <v>9</v>
+      </c>
       <c r="K174" s="20">
         <v>73.3</v>
       </c>
@@ -11695,7 +12559,9 @@
       <c r="I175" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J175" s="14"/>
+      <c r="J175" s="14">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="K175" s="20">
         <v>73.3</v>
       </c>
@@ -11747,7 +12613,9 @@
       <c r="I176" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J176" s="14"/>
+      <c r="J176" s="14">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="K176" s="20">
         <v>73.3</v>
       </c>
@@ -11799,7 +12667,9 @@
       <c r="I177" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="J177" s="14"/>
+      <c r="J177" s="14">
+        <v>10.5</v>
+      </c>
       <c r="K177" s="20">
         <v>73.3</v>
       </c>
@@ -11851,7 +12721,9 @@
       <c r="I178" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="J178" s="14"/>
+      <c r="J178" s="14">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="K178" s="20">
         <v>73.3</v>
       </c>
@@ -11903,7 +12775,9 @@
       <c r="I179" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J179" s="14"/>
+      <c r="J179" s="14">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="K179" s="20">
         <v>44.4</v>
       </c>
@@ -11955,7 +12829,9 @@
       <c r="I180" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J180" s="14"/>
+      <c r="J180" s="14">
+        <v>7.6</v>
+      </c>
       <c r="K180" s="20">
         <v>44.4</v>
       </c>
@@ -12007,7 +12883,9 @@
       <c r="I181" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J181" s="14"/>
+      <c r="J181" s="14">
+        <v>8.4</v>
+      </c>
       <c r="K181" s="20">
         <v>44.4</v>
       </c>
@@ -12059,7 +12937,9 @@
       <c r="I182" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J182" s="14"/>
+      <c r="J182" s="14">
+        <v>8.4</v>
+      </c>
       <c r="K182" s="20">
         <v>44.4</v>
       </c>
@@ -12111,7 +12991,9 @@
       <c r="I183" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="J183" s="14"/>
+      <c r="J183" s="14">
+        <v>5.8</v>
+      </c>
       <c r="K183" s="20">
         <v>44.4</v>
       </c>
@@ -12164,7 +13046,9 @@
       <c r="I184" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="J184" s="14"/>
+      <c r="J184" s="14">
+        <v>6.4</v>
+      </c>
       <c r="K184" s="20">
         <v>44.4</v>
       </c>
@@ -12216,7 +13100,9 @@
       <c r="I185" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J185" s="14"/>
+      <c r="J185" s="14">
+        <v>6.7</v>
+      </c>
       <c r="K185" s="20">
         <v>14</v>
       </c>
@@ -12268,7 +13154,9 @@
       <c r="I186" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J186" s="14"/>
+      <c r="J186" s="14">
+        <v>6.7</v>
+      </c>
       <c r="K186" s="20">
         <v>14</v>
       </c>
@@ -12320,7 +13208,9 @@
       <c r="I187" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J187" s="14"/>
+      <c r="J187" s="14">
+        <v>15.4</v>
+      </c>
       <c r="K187" s="20">
         <v>14</v>
       </c>
@@ -12372,7 +13262,9 @@
       <c r="I188" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J188" s="14"/>
+      <c r="J188" s="14">
+        <v>15.4</v>
+      </c>
       <c r="K188" s="20">
         <v>14</v>
       </c>
@@ -12424,7 +13316,9 @@
       <c r="I189" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="J189" s="14"/>
+      <c r="J189" s="14">
+        <v>7.9</v>
+      </c>
       <c r="K189" s="20">
         <v>14</v>
       </c>
@@ -12476,7 +13370,9 @@
       <c r="I190" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="J190" s="14"/>
+      <c r="J190" s="14">
+        <v>7.9</v>
+      </c>
       <c r="K190" s="20">
         <v>14</v>
       </c>
@@ -12528,7 +13424,9 @@
       <c r="I191" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="J191" s="14"/>
+      <c r="J191" s="14">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="K191" s="20">
         <v>14</v>
       </c>
@@ -12580,7 +13478,9 @@
       <c r="I192" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="J192" s="14"/>
+      <c r="J192" s="14">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="K192" s="20">
         <v>14</v>
       </c>
@@ -12632,7 +13532,9 @@
       <c r="I193" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J193" s="14"/>
+      <c r="J193" s="14">
+        <v>6.8</v>
+      </c>
       <c r="K193" s="20">
         <v>14</v>
       </c>
@@ -12685,7 +13587,9 @@
       <c r="I194" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J194" s="14"/>
+      <c r="J194" s="14">
+        <v>11.1</v>
+      </c>
       <c r="K194" s="20">
         <v>14</v>
       </c>
@@ -12738,7 +13642,9 @@
       <c r="I195" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="J195" s="14"/>
+      <c r="J195" s="14">
+        <v>3.7</v>
+      </c>
       <c r="K195" s="20">
         <v>14</v>
       </c>
@@ -12790,7 +13696,9 @@
       <c r="I196" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="J196" s="14"/>
+      <c r="J196" s="14">
+        <v>6.4</v>
+      </c>
       <c r="K196" s="20">
         <v>14</v>
       </c>
@@ -12842,7 +13750,9 @@
       <c r="I197" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J197" s="14"/>
+      <c r="J197" s="14">
+        <v>6.5</v>
+      </c>
       <c r="K197" s="20">
         <v>12.4</v>
       </c>
@@ -12894,7 +13804,9 @@
       <c r="I198" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J198" s="14"/>
+      <c r="J198" s="14">
+        <v>6.5</v>
+      </c>
       <c r="K198" s="20">
         <v>12.4</v>
       </c>
@@ -12946,7 +13858,9 @@
       <c r="I199" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J199" s="14"/>
+      <c r="J199" s="14">
+        <v>8.5</v>
+      </c>
       <c r="K199" s="20">
         <v>12.4</v>
       </c>
@@ -12998,7 +13912,9 @@
       <c r="I200" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J200" s="14"/>
+      <c r="J200" s="14">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="K200" s="20">
         <v>12.4</v>
       </c>
@@ -13050,7 +13966,9 @@
       <c r="I201" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="J201" s="14"/>
+      <c r="J201" s="14">
+        <v>9.6</v>
+      </c>
       <c r="K201" s="20">
         <v>12.4</v>
       </c>
@@ -13102,7 +14020,9 @@
       <c r="I202" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="J202" s="14"/>
+      <c r="J202" s="14">
+        <v>7.5</v>
+      </c>
       <c r="K202" s="20">
         <v>12.4</v>
       </c>
@@ -13154,7 +14074,9 @@
       <c r="I203" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J203" s="14"/>
+      <c r="J203" s="14">
+        <v>7.3</v>
+      </c>
       <c r="K203" s="20">
         <v>12.4</v>
       </c>
@@ -13206,7 +14128,9 @@
       <c r="I204" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="J204" s="14"/>
+      <c r="J204" s="14">
+        <v>7.6</v>
+      </c>
       <c r="K204" s="20">
         <v>12.4</v>
       </c>
@@ -13258,7 +14182,9 @@
       <c r="I205" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J205" s="14"/>
+      <c r="J205" s="14">
+        <v>10.6</v>
+      </c>
       <c r="K205" s="20">
         <v>12.4</v>
       </c>
@@ -13311,7 +14237,9 @@
       <c r="I206" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J206" s="14"/>
+      <c r="J206" s="14">
+        <v>10.6</v>
+      </c>
       <c r="K206" s="20">
         <v>12.4</v>
       </c>
@@ -13364,7 +14292,9 @@
       <c r="I207" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="J207" s="14"/>
+      <c r="J207" s="14">
+        <v>11.4</v>
+      </c>
       <c r="K207" s="20">
         <v>12.4</v>
       </c>
@@ -13416,7 +14346,9 @@
       <c r="I208" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="J208" s="14"/>
+      <c r="J208" s="14">
+        <v>11.4</v>
+      </c>
       <c r="K208" s="20">
         <v>12.4</v>
       </c>
@@ -13468,7 +14400,9 @@
       <c r="I209" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J209" s="14"/>
+      <c r="J209" s="14">
+        <v>5.6</v>
+      </c>
       <c r="K209" s="20">
         <v>16.3</v>
       </c>
@@ -13521,7 +14455,9 @@
       <c r="I210" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J210" s="14"/>
+      <c r="J210" s="14">
+        <v>5.6</v>
+      </c>
       <c r="K210" s="20">
         <v>16.3</v>
       </c>
@@ -13574,7 +14510,9 @@
       <c r="I211" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J211" s="14"/>
+      <c r="J211" s="14">
+        <v>4.8</v>
+      </c>
       <c r="K211" s="20">
         <v>16.3</v>
       </c>
@@ -13626,7 +14564,9 @@
       <c r="I212" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J212" s="14"/>
+      <c r="J212" s="14">
+        <v>4.8</v>
+      </c>
       <c r="K212" s="20">
         <v>16.3</v>
       </c>
@@ -13679,7 +14619,9 @@
       <c r="I213" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="J213" s="14"/>
+      <c r="J213" s="14">
+        <v>5.7</v>
+      </c>
       <c r="K213" s="20">
         <v>16.3</v>
       </c>
@@ -13731,7 +14673,9 @@
       <c r="I214" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="J214" s="14"/>
+      <c r="J214" s="14">
+        <v>5.7</v>
+      </c>
       <c r="K214" s="20">
         <v>16.3</v>
       </c>
@@ -13783,7 +14727,9 @@
       <c r="I215" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="J215" s="14"/>
+      <c r="J215" s="14">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="K215" s="20">
         <v>1282</v>
       </c>
@@ -13836,7 +14782,9 @@
       <c r="I216" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J216" s="14"/>
+      <c r="J216" s="14">
+        <v>5.5</v>
+      </c>
       <c r="K216" s="20">
         <v>1282</v>
       </c>
@@ -13889,7 +14837,9 @@
       <c r="I217" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J217" s="14"/>
+      <c r="J217" s="14">
+        <v>7.8</v>
+      </c>
       <c r="K217" s="20">
         <v>1282</v>
       </c>
@@ -13941,7 +14891,9 @@
       <c r="I218" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J218" s="14"/>
+      <c r="J218" s="14">
+        <v>7.8</v>
+      </c>
       <c r="K218" s="20">
         <v>1282</v>
       </c>
@@ -13994,7 +14946,9 @@
       <c r="I219" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="J219" s="14"/>
+      <c r="J219" s="14">
+        <v>6.2</v>
+      </c>
       <c r="K219" s="20">
         <v>1282</v>
       </c>
@@ -14047,7 +15001,9 @@
       <c r="I220" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="J220" s="14"/>
+      <c r="J220" s="14">
+        <v>8.4</v>
+      </c>
       <c r="K220" s="20">
         <v>1282</v>
       </c>
@@ -14099,7 +15055,9 @@
       <c r="I221" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J221" s="14"/>
+      <c r="J221" s="14">
+        <v>8.5</v>
+      </c>
       <c r="K221" s="20">
         <v>2.17</v>
       </c>
@@ -14151,7 +15109,9 @@
       <c r="I222" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J222" s="14"/>
+      <c r="J222" s="14">
+        <v>8.5</v>
+      </c>
       <c r="K222" s="20">
         <v>2.17</v>
       </c>
@@ -14204,7 +15164,9 @@
       <c r="I223" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J223" s="14"/>
+      <c r="J223" s="14">
+        <v>7.3</v>
+      </c>
       <c r="K223" s="20">
         <v>2.17</v>
       </c>
@@ -14256,7 +15218,9 @@
       <c r="I224" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J224" s="14"/>
+      <c r="J224" s="14">
+        <v>7.3</v>
+      </c>
       <c r="K224" s="20">
         <v>2.17</v>
       </c>
@@ -14308,7 +15272,9 @@
       <c r="I225" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="J225" s="14"/>
+      <c r="J225" s="14">
+        <v>8</v>
+      </c>
       <c r="K225" s="20">
         <v>2.17</v>
       </c>
@@ -14360,7 +15326,9 @@
       <c r="I226" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="J226" s="14"/>
+      <c r="J226" s="14">
+        <v>8</v>
+      </c>
       <c r="K226" s="20">
         <v>2.17</v>
       </c>
@@ -14413,7 +15381,9 @@
       <c r="I227" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J227" s="14"/>
+      <c r="J227" s="14">
+        <v>6.3</v>
+      </c>
       <c r="K227" s="20">
         <v>1.59</v>
       </c>
@@ -14465,7 +15435,9 @@
       <c r="I228" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J228" s="14"/>
+      <c r="J228" s="14">
+        <v>6.3</v>
+      </c>
       <c r="K228" s="20">
         <v>1.59</v>
       </c>
@@ -14517,7 +15489,9 @@
       <c r="I229" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J229" s="14"/>
+      <c r="J229" s="14">
+        <v>7</v>
+      </c>
       <c r="K229" s="20">
         <v>1.59</v>
       </c>
@@ -14569,7 +15543,9 @@
       <c r="I230" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J230" s="14"/>
+      <c r="J230" s="14">
+        <v>7.5</v>
+      </c>
       <c r="K230" s="20">
         <v>1.59</v>
       </c>
@@ -14621,7 +15597,9 @@
       <c r="I231" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="J231" s="14"/>
+      <c r="J231" s="14">
+        <v>7.2</v>
+      </c>
       <c r="K231" s="20">
         <v>1.59</v>
       </c>
@@ -14673,7 +15651,9 @@
       <c r="I232" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="J232" s="14"/>
+      <c r="J232" s="14">
+        <v>7.2</v>
+      </c>
       <c r="K232" s="20">
         <v>1.59</v>
       </c>
@@ -14725,7 +15705,9 @@
       <c r="I233" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J233" s="14"/>
+      <c r="J233" s="14">
+        <v>8</v>
+      </c>
       <c r="K233" s="20">
         <v>108</v>
       </c>
@@ -14777,7 +15759,9 @@
       <c r="I234" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J234" s="14"/>
+      <c r="J234" s="14">
+        <v>8</v>
+      </c>
       <c r="K234" s="20">
         <v>108</v>
       </c>
@@ -14829,7 +15813,9 @@
       <c r="I235" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J235" s="14"/>
+      <c r="J235" s="14">
+        <v>7.1</v>
+      </c>
       <c r="K235" s="20">
         <v>108</v>
       </c>
@@ -14881,7 +15867,9 @@
       <c r="I236" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="J236" s="14"/>
+      <c r="J236" s="14">
+        <v>7.1</v>
+      </c>
       <c r="K236" s="20">
         <v>108</v>
       </c>
@@ -14933,7 +15921,9 @@
       <c r="I237" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="J237" s="14"/>
+      <c r="J237" s="14">
+        <v>10.5</v>
+      </c>
       <c r="K237" s="20">
         <v>108</v>
       </c>
@@ -14985,7 +15975,9 @@
       <c r="I238" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="J238" s="14"/>
+      <c r="J238" s="14">
+        <v>5.9</v>
+      </c>
       <c r="K238" s="20">
         <v>108</v>
       </c>
@@ -15037,7 +16029,9 @@
       <c r="I239" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="J239" s="14"/>
+      <c r="J239" s="14">
+        <v>5.5</v>
+      </c>
       <c r="K239" s="20">
         <v>108</v>
       </c>
@@ -15089,7 +16083,9 @@
       <c r="I240" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="J240" s="14"/>
+      <c r="J240" s="14">
+        <v>5.5</v>
+      </c>
       <c r="K240" s="20">
         <v>108</v>
       </c>
@@ -15141,7 +16137,9 @@
       <c r="I241" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J241" s="14"/>
+      <c r="J241" s="14">
+        <v>8.1</v>
+      </c>
       <c r="K241" s="20">
         <v>108</v>
       </c>
@@ -15193,7 +16191,9 @@
       <c r="I242" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J242" s="14"/>
+      <c r="J242" s="14">
+        <v>8.1</v>
+      </c>
       <c r="K242" s="20">
         <v>108</v>
       </c>
@@ -15245,7 +16245,9 @@
       <c r="I243" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="J243" s="14"/>
+      <c r="J243" s="14">
+        <v>6.5</v>
+      </c>
       <c r="K243" s="20">
         <v>108</v>
       </c>
@@ -15297,7 +16299,9 @@
       <c r="I244" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="J244" s="14"/>
+      <c r="J244" s="14">
+        <v>5.7</v>
+      </c>
       <c r="K244" s="20">
         <v>108</v>
       </c>
@@ -15349,7 +16353,9 @@
       <c r="I245" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J245" s="14"/>
+      <c r="J245" s="14">
+        <v>18</v>
+      </c>
       <c r="K245" s="20">
         <v>12.3</v>
       </c>
@@ -15401,7 +16407,9 @@
       <c r="I246" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J246" s="14"/>
+      <c r="J246" s="14">
+        <v>18</v>
+      </c>
       <c r="K246" s="20">
         <v>12.3</v>
       </c>
@@ -15453,7 +16461,9 @@
       <c r="I247" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J247" s="14"/>
+      <c r="J247" s="14">
+        <v>12.1</v>
+      </c>
       <c r="K247" s="20">
         <v>12.3</v>
       </c>
@@ -15505,7 +16515,9 @@
       <c r="I248" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="J248" s="14"/>
+      <c r="J248" s="14">
+        <v>8.1</v>
+      </c>
       <c r="K248" s="20">
         <v>12.3</v>
       </c>
@@ -15557,7 +16569,9 @@
       <c r="I249" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="J249" s="14"/>
+      <c r="J249" s="14">
+        <v>11.2</v>
+      </c>
       <c r="K249" s="20">
         <v>12.3</v>
       </c>
@@ -15610,7 +16624,9 @@
       <c r="I250" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="J250" s="14"/>
+      <c r="J250" s="14">
+        <v>11.2</v>
+      </c>
       <c r="K250" s="20">
         <v>12.3</v>
       </c>
@@ -15663,7 +16679,9 @@
       <c r="I251" s="40" t="s">
         <v>324</v>
       </c>
-      <c r="J251" s="15"/>
+      <c r="J251" s="15">
+        <v>9.6</v>
+      </c>
       <c r="K251" s="41">
         <v>2.72</v>
       </c>
@@ -15715,7 +16733,9 @@
       <c r="I252" s="40" t="s">
         <v>320</v>
       </c>
-      <c r="J252" s="15"/>
+      <c r="J252" s="15">
+        <v>10.8</v>
+      </c>
       <c r="K252" s="41">
         <v>2.72</v>
       </c>
@@ -15766,7 +16786,9 @@
       <c r="I253" s="40" t="s">
         <v>321</v>
       </c>
-      <c r="J253" s="15"/>
+      <c r="J253" s="15">
+        <v>11.2</v>
+      </c>
       <c r="K253" s="41">
         <v>2.72</v>
       </c>
@@ -15817,7 +16839,9 @@
       <c r="I254" s="40" t="s">
         <v>321</v>
       </c>
-      <c r="J254" s="15"/>
+      <c r="J254" s="15">
+        <v>11.2</v>
+      </c>
       <c r="K254" s="41">
         <v>2.72</v>
       </c>
@@ -15868,7 +16892,9 @@
       <c r="I255" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="J255" s="15"/>
+      <c r="J255" s="15">
+        <v>25.9</v>
+      </c>
       <c r="K255" s="41">
         <v>2.72</v>
       </c>
@@ -15919,7 +16945,9 @@
       <c r="I256" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="J256" s="15"/>
+      <c r="J256" s="15">
+        <v>25.9</v>
+      </c>
       <c r="K256" s="41">
         <v>2.72</v>
       </c>
@@ -15956,16 +16984,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BB9379-2E49-1147-9B3F-79136290B7F5}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.15">
@@ -16046,6 +17075,196 @@
         <v>342</v>
       </c>
     </row>
+    <row r="18" spans="2:3" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="C18" s="58"/>
+    </row>
+    <row r="19" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="59" t="s">
+        <v>349</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="61" t="s">
+        <v>351</v>
+      </c>
+      <c r="C20" s="62" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="61" t="s">
+        <v>353</v>
+      </c>
+      <c r="C21" s="62" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="61" t="s">
+        <v>355</v>
+      </c>
+      <c r="C22" s="62" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="61" t="s">
+        <v>357</v>
+      </c>
+      <c r="C23" s="62" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="61" t="s">
+        <v>359</v>
+      </c>
+      <c r="C24" s="62" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="63" t="s">
+        <v>361</v>
+      </c>
+      <c r="C25" s="62" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="61" t="s">
+        <v>363</v>
+      </c>
+      <c r="C26" s="62" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="61" t="s">
+        <v>365</v>
+      </c>
+      <c r="C27" s="62" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="61" t="s">
+        <v>367</v>
+      </c>
+      <c r="C28" s="62" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="61" t="s">
+        <v>369</v>
+      </c>
+      <c r="C29" s="62" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="61" t="s">
+        <v>371</v>
+      </c>
+      <c r="C30" s="62" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="61" t="s">
+        <v>373</v>
+      </c>
+      <c r="C31" s="62" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="61" t="s">
+        <v>375</v>
+      </c>
+      <c r="C32" s="62" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="64" t="s">
+        <v>377</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34" s="61" t="s">
+        <v>379</v>
+      </c>
+      <c r="C34" s="62" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B35" s="61" t="s">
+        <v>381</v>
+      </c>
+      <c r="C35" s="62" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36" s="61" t="s">
+        <v>383</v>
+      </c>
+      <c r="C36" s="62" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B37" s="61" t="s">
+        <v>385</v>
+      </c>
+      <c r="C37" s="62" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="61" t="s">
+        <v>387</v>
+      </c>
+      <c r="C38" s="62" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39" s="61" t="s">
+        <v>389</v>
+      </c>
+      <c r="C39" s="62" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40" s="61" t="s">
+        <v>391</v>
+      </c>
+      <c r="C40" s="62" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="61" t="s">
+        <v>393</v>
+      </c>
+      <c r="C41" s="62" t="s">
+        <v>394</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>